<commit_message>
logo responsive et modification du nom de la page 2
</commit_message>
<xml_diff>
--- a/Copie de Modele-audit-SEO.xlsx
+++ b/Copie de Modele-audit-SEO.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="81">
   <si>
     <t>Catégorie</t>
   </si>
@@ -73,45 +73,21 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>pas de titre sur onglet</t>
-  </si>
-  <si>
-    <t>un point sur la balise Title au lieu du nom</t>
-  </si>
-  <si>
     <t>Page</t>
   </si>
   <si>
     <t>SEO</t>
   </si>
   <si>
-    <t>"page 2" au lieu d'un titre</t>
-  </si>
-  <si>
-    <t>mauvais nom d'onglet</t>
-  </si>
-  <si>
-    <t>Mettre le nom de l'agence</t>
-  </si>
-  <si>
     <t>valeur attribut "lang" balise &lt;html&gt; en "défaut"</t>
   </si>
   <si>
-    <t>l'attribut "lang" doit etre defini par une langue</t>
-  </si>
-  <si>
-    <t>balise meta keyword</t>
-  </si>
-  <si>
     <t>à supprimer</t>
   </si>
   <si>
     <t>balise meta description, content vide</t>
   </si>
   <si>
-    <t>mettre une description</t>
-  </si>
-  <si>
     <t>balises scriptS L15 à L19</t>
   </si>
   <si>
@@ -130,15 +106,6 @@
     <t>mettre fr car site en français</t>
   </si>
   <si>
-    <t>manque H2 dans structure titre</t>
-  </si>
-  <si>
-    <t>il faut un H2 avant un H3</t>
-  </si>
-  <si>
-    <t>restructurer les titres dans l'ordre</t>
-  </si>
-  <si>
     <t>alt des images non correspondantes</t>
   </si>
   <si>
@@ -148,9 +115,6 @@
     <t>modifier les alt</t>
   </si>
   <si>
-    <t>images trop grandes</t>
-  </si>
-  <si>
     <t>images plus grande que leur conteneurs</t>
   </si>
   <si>
@@ -160,15 +124,6 @@
     <t>1 et 2</t>
   </si>
   <si>
-    <t>contraste</t>
-  </si>
-  <si>
-    <t>validation de contraste</t>
-  </si>
-  <si>
-    <t>réadapter les contrastes</t>
-  </si>
-  <si>
     <t>texte à 1px</t>
   </si>
   <si>
@@ -196,12 +151,6 @@
     <t>rien ne ressort dans le css et le site</t>
   </si>
   <si>
-    <t>lien inutile qui rafraîchit alors que logo le fait déjà</t>
-  </si>
-  <si>
-    <t>2 renvoie ''liens'' sur la page index</t>
-  </si>
-  <si>
     <t>Lien accueil et page 2 tout à droite qui est inutile</t>
   </si>
   <si>
@@ -211,18 +160,12 @@
     <t>supp</t>
   </si>
   <si>
-    <t>mettre le nom ''contact'' comme nom de page</t>
-  </si>
-  <si>
     <t>&amp; alors que il y le charset utf 8</t>
   </si>
   <si>
     <t>Meta charset utf 8 pour l'encodage des caractères</t>
   </si>
   <si>
-    <t>à remplacer</t>
-  </si>
-  <si>
     <t>liens vide pour les réseaux sociaux</t>
   </si>
   <si>
@@ -260,13 +203,106 @@
   </si>
   <si>
     <t>https://www.anthedesign.fr/referencement/backlink/#:~:text=Obtenir%20des%20backlinks%20de%20qualit%C3%A9,page%20similaire%20sans%20liens%20entrants.</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/International/questions/qa-html-language-declarations.fr</t>
+  </si>
+  <si>
+    <t>l'attribut "lang" doit être défini par une langue</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>balise meta keyword avec spam de mot clefs</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/la-balise-meta-keywords/</t>
+  </si>
+  <si>
+    <t>mettre une description attractive pour le site</t>
+  </si>
+  <si>
+    <t>https://optimiz.me/metadonnee-description-2/</t>
+  </si>
+  <si>
+    <t>La balise title défini le nom de la page</t>
+  </si>
+  <si>
+    <t>https://www.definitions-seo.com/definition-de-balise-title/#:~:text=La%20Balise%20Title%20est%20une,la%20page%20par%20Google…</t>
+  </si>
+  <si>
+    <t>https://www.jchr.be/html/caracteres.htm</t>
+  </si>
+  <si>
+    <t>à remplacer par la meta charset utf-8 car l'esperluette n'est plus utilisé pour l'encodage des caractères spéciaux</t>
+  </si>
+  <si>
+    <t>Les balises title des page n'étaient nommée correctement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre un titre pertinent pour les deux pages </t>
+  </si>
+  <si>
+    <t>à supprimer car cette balise n'est plus pris en compte par les robots des moteurs de recherche car utilisé abusivement avant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">black hat car spam de mots clefs </t>
+  </si>
+  <si>
+    <t>Pas de balises sémentiques et mauvaise structure du code HTML</t>
+  </si>
+  <si>
+    <t>Les balises sémentiques manquantes et l'ordre des H (h1,h2) n'étaient pas appliqué</t>
+  </si>
+  <si>
+    <t>restructurer les balises et ajouté quelques balises sémentiques</t>
+  </si>
+  <si>
+    <t>fait</t>
+  </si>
+  <si>
+    <t>Accessibilité</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/html/html5_semantic_elements.asp</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>Les images sont trop lourdes</t>
+  </si>
+  <si>
+    <t>Pour optimisé les performances j'ai compressé et converti les images</t>
+  </si>
+  <si>
+    <t>https://yesyouweb.com/pourquoi-comment-optimiser-images-site-web/</t>
+  </si>
+  <si>
+    <t>Quelques textes sont invisibles et autres texte avec un mauvais ratio de contrast</t>
+  </si>
+  <si>
+    <t>Les texte invisibles sont du blackhat car ils avaient des spam de keyword</t>
+  </si>
+  <si>
+    <t>Avoir des couleurs avec un bon ratio de contrast, et effacé les texte invisibles car c'est du blackhat à ne pas faire</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
+  </si>
+  <si>
+    <t>accessibilité</t>
+  </si>
+  <si>
+    <t>google search console  avec les mots clefs et le traffic pour le cdn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,11 +325,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -311,6 +342,25 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -345,9 +395,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -357,20 +407,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -389,9 +445,27 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -407,9 +481,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -425,9 +499,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -443,9 +517,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -461,9 +535,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -479,9 +553,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -497,27 +571,9 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
+        <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -560,16 +616,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G24" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:G22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="0">
+  <autoFilter ref="A1:G22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Page" dataDxfId="6"/>
-    <tableColumn id="2" name="Catégorie" dataDxfId="5"/>
-    <tableColumn id="3" name="Problème identifié" dataDxfId="4"/>
-    <tableColumn id="4" name="Explication du problème" dataDxfId="3"/>
-    <tableColumn id="5" name="Bonne pratique à adopter" dataDxfId="2"/>
-    <tableColumn id="6" name="Action recommandée" dataDxfId="1"/>
-    <tableColumn id="7" name="Référence" dataDxfId="0"/>
+    <tableColumn id="1" name="Page" dataDxfId="7"/>
+    <tableColumn id="2" name="Catégorie" dataDxfId="6"/>
+    <tableColumn id="3" name="Problème identifié" dataDxfId="5"/>
+    <tableColumn id="4" name="Explication du problème" dataDxfId="4"/>
+    <tableColumn id="5" name="Bonne pratique à adopter" dataDxfId="3"/>
+    <tableColumn id="6" name="Action recommandée" dataDxfId="2"/>
+    <tableColumn id="7" name="Référence" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -773,26 +829,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1008"/>
+  <dimension ref="A1:AA1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="63.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" customWidth="1"/>
     <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="28.5546875" customWidth="1"/>
+    <col min="7" max="7" width="42.33203125" customWidth="1"/>
     <col min="8" max="27" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -833,454 +890,440 @@
       <c r="Z1" s="1"/>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" s="4" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:27" s="4" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" s="4" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:27" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>1</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:27" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>1</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>2</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="F21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:9" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:27" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>1</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:27" ht="45" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>1</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="F22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>1</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>1</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>1</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>1</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>2</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
-        <v>2</v>
-      </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6"/>
-      <c r="I23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="11" t="s">
+        <v>80</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1298,33 +1341,17 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+    </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
-    </row>
+    <row r="36" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1516,13 +1543,13 @@
     <row r="225" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="226" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="227" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C228" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="229" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C230" t="s">
-        <v>42</v>
-      </c>
-    </row>
+    <row r="230" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="231" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="232" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="233" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2299,18 +2326,24 @@
     <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G12" r:id="rId1"/>
+    <hyperlink ref="G11" r:id="rId1"/>
     <hyperlink ref="G4" r:id="rId2" location=":~:text=Obtenir%20des%20backlinks%20de%20qualit%C3%A9,page%20similaire%20sans%20liens%20entrants."/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId6" location=":~:text=La%20Balise%20Title%20est%20une,la%20page%20par%20Google…"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="G9" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId9"/>
+    <hyperlink ref="G13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dernière modification de l'audit
</commit_message>
<xml_diff>
--- a/Copie de Modele-audit-SEO.xlsx
+++ b/Copie de Modele-audit-SEO.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
   <si>
     <t>Catégorie</t>
   </si>
@@ -79,15 +79,9 @@
     <t>valeur attribut "lang" balise &lt;html&gt; en "défaut"</t>
   </si>
   <si>
-    <t>balise meta description, content vide</t>
-  </si>
-  <si>
     <t>balises scriptS L15 à L19</t>
   </si>
   <si>
-    <t>il faut une description, phrase d'accroche</t>
-  </si>
-  <si>
     <t>mettre "async" ou "defer"</t>
   </si>
   <si>
@@ -160,30 +154,15 @@
     <t>https://optimiz.me/la-balise-meta-keywords/</t>
   </si>
   <si>
-    <t>mettre une description attractive pour le site</t>
-  </si>
-  <si>
     <t>https://optimiz.me/metadonnee-description-2/</t>
   </si>
   <si>
-    <t>La balise title défini le nom de la page</t>
-  </si>
-  <si>
-    <t>https://www.definitions-seo.com/definition-de-balise-title/#:~:text=La%20Balise%20Title%20est%20une,la%20page%20par%20Google…</t>
-  </si>
-  <si>
     <t>https://www.jchr.be/html/caracteres.htm</t>
   </si>
   <si>
     <t>à remplacer par la meta charset utf-8 car l'esperluette n'est plus utilisé pour l'encodage des caractères spéciaux</t>
   </si>
   <si>
-    <t>Les balises title des page n'étaient nommée correctement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mettre un titre pertinent pour les deux pages </t>
-  </si>
-  <si>
     <t>à supprimer car cette balise n'est plus pris en compte par les robots des moteurs de recherche car utilisé abusivement avant</t>
   </si>
   <si>
@@ -238,9 +217,6 @@
     <t>Il faut avoir de bon liens et qu'ils soient cohérent avec le théme du site</t>
   </si>
   <si>
-    <t>La meta description est importante faut en avoir une pour avoir un bon référencement de la page</t>
-  </si>
-  <si>
     <t>redimmensionné ou compressé les images pour plus de performance</t>
   </si>
   <si>
@@ -250,9 +226,6 @@
     <t>Il faut avoir une bonne description d'image pour le SEO et l'accéssibilité</t>
   </si>
   <si>
-    <t xml:space="preserve">Avoir un titre cohérent avec le site </t>
-  </si>
-  <si>
     <t>Avoir un charset utf 8 permettra d'encoder les caractères correctement</t>
   </si>
   <si>
@@ -320,6 +293,21 @@
   </si>
   <si>
     <t>Les liens ne sont pas cohérent avec l'entreprise</t>
+  </si>
+  <si>
+    <t>balise meta description, content vide également pour le title de la page</t>
+  </si>
+  <si>
+    <t>SEO et bonne pratique</t>
+  </si>
+  <si>
+    <t>il faut une description, phrase d'accroche et définir le nom de la page</t>
+  </si>
+  <si>
+    <t>mettre une description attractive pour le site et définir le titre des pages avec la balise title</t>
+  </si>
+  <si>
+    <t>La meta description est importante faut en avoir une pour avoir un bon référencement de la page, la balise title est importante lors de la recherche du site sur internet.</t>
   </si>
 </sst>
 </file>
@@ -906,7 +894,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -962,22 +950,22 @@
     </row>
     <row r="2" spans="1:26" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,99 +973,99 @@
         <v>6</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="E4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="B6" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>38</v>
+      <c r="D6" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="4" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1085,79 +1073,79 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="E9" s="10" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
@@ -1165,39 +1153,39 @@
         <v>6</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1205,77 +1193,57 @@
         <v>6</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="E14" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -2326,22 +2294,21 @@
     <hyperlink ref="F2" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4"/>
     <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6" location=":~:text=La%20Balise%20Title%20est%20une,la%20page%20par%20Google…"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F10" r:id="rId8"/>
-    <hyperlink ref="F7" r:id="rId9"/>
-    <hyperlink ref="F9" r:id="rId10"/>
-    <hyperlink ref="F17" r:id="rId11"/>
-    <hyperlink ref="F11" r:id="rId12"/>
-    <hyperlink ref="F16" r:id="rId13"/>
-    <hyperlink ref="F13" r:id="rId14"/>
-    <hyperlink ref="F15" r:id="rId15"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="F7" r:id="rId8"/>
+    <hyperlink ref="F9" r:id="rId9"/>
+    <hyperlink ref="F17" r:id="rId10"/>
+    <hyperlink ref="F11" r:id="rId11"/>
+    <hyperlink ref="F6" r:id="rId12"/>
+    <hyperlink ref="F13" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId16"/>
-  <legacyDrawing r:id="rId17"/>
+  <pageSetup orientation="landscape" r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>